<commit_message>
Add POS Detail to excel sheet for Wire Pu Rann
</commit_message>
<xml_diff>
--- a/bin/Debug/Template/SDCalcForProduction_Template.xlsx
+++ b/bin/Debug/Template/SDCalcForProduction_Template.xlsx
@@ -5,18 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Current Works\MachineDeptApp v1.0.0.8\Source Code\bin\Debug\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Current Works\MC-Dept-App\bin\Debug\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8B3D3B-C80D-478C-9D2A-813E7009BFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CCAB55-5E57-4272-AACD-A9B858696236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{14D0DD05-F513-4696-888A-6119A7C86A21}"/>
   </bookViews>
   <sheets>
     <sheet name="RachhanSystem" sheetId="1" r:id="rId1"/>
+    <sheet name="POSList" sheetId="3" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">POSList!$A$3:$G$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RachhanSystem!$A$5:$C$5</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="SK_A20">[1]Memo!$J$2+[1]Memo!$J$2:$J$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>លេខកូដ</t>
   </si>
@@ -49,6 +56,49 @@
   </si>
   <si>
     <t>ទិន្នន័យវេរទៅផលិត</t>
+  </si>
+  <si>
+    <t>SEMI CODE</t>
+    <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>Semi Name</t>
+    <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>POS( C )</t>
+    <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>Pin Assignment</t>
+  </si>
+  <si>
+    <t>Wire/Tube Color</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Qty</t>
+    <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>លេខកូដ Semi</t>
+  </si>
+  <si>
+    <t>ឈ្មោះ Semi</t>
+  </si>
+  <si>
+    <t>POS( C )</t>
+  </si>
+  <si>
+    <t>ភីន</t>
+  </si>
+  <si>
+    <t>ពណ៌ខ្សែភ្លើង</t>
+  </si>
+  <si>
+    <t>ប្រវែង</t>
   </si>
 </sst>
 </file>
@@ -59,7 +109,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,8 +142,45 @@
       <color theme="1"/>
       <name val="Khmer OS Battambang"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Khmer OS Battambang"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Khmer OS Battambang"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,8 +193,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -220,11 +319,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -251,20 +404,198 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="6" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="6" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="6" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
+    <xf numFmtId="38" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comma [0] 2" xfId="2" xr:uid="{AD6CEE88-2E7A-43E7-8791-B21BC8C3A6F0}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{0C4DE3D2-7F48-4CEA-A796-6055F961D19F}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF87CEEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC0CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF008000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADFF2F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA52A2A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0000FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC0CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -603,6 +934,35 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Memo"/>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="J2" t="str">
+            <v>SK-A20 (A)</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="J3" t="str">
+            <v>SK-A20 (B)</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -911,35 +1271,35 @@
       <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="56" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:3" ht="40.5" customHeight="1">
+      <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="26.25" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="str">
         <f>IF(A2&lt;&gt;""," ៖ "&amp;TEXT(A2,"dd-MM-yyyy")," ៖ ")</f>
         <v xml:space="preserve"> ៖ </v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="26.25" customHeight="1" thickBot="1">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="str">
         <f>IF(A3&lt;&gt;""," ៖ "&amp;A3," ៖ ")</f>
         <v xml:space="preserve"> ៖ </v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:3" ht="23.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -950,7 +1310,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:3" ht="24" thickBot="1">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -961,10 +1321,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+    <row r="6" spans="1:3" ht="23.25">
+      <c r="A6" s="10"/>
       <c r="B6" s="9"/>
-      <c r="C6" s="12"/>
+      <c r="C6" s="11"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:C5" xr:uid="{7D00B6B8-4ABD-4A98-AC4F-01406F7FAE6A}"/>
@@ -979,4 +1339,144 @@
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3D4DE8-B852-41EA-96A7-EF1788C15BF6}">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.249977111117893"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:AP4"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="29" style="13" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" style="13" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:7" s="19" customFormat="1" ht="19.5">
+      <c r="A2" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="19" customFormat="1" ht="20.25" thickBot="1">
+      <c r="A3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="27" customFormat="1" ht="18" customHeight="1">
+      <c r="A4" s="23"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="24"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A3:G3" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <conditionalFormatting sqref="E2:E4">
+    <cfRule type="containsText" dxfId="12" priority="13" stopIfTrue="1" operator="containsText" text="RED">
+      <formula>NOT(ISERROR(SEARCH("RED",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="14" stopIfTrue="1" operator="containsText" text="BLK">
+      <formula>NOT(ISERROR(SEARCH("BLK",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="15" stopIfTrue="1" operator="containsText" text="PINK">
+      <formula>NOT(ISERROR(SEARCH("PINK",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="16" stopIfTrue="1" operator="containsText" text="YEL">
+      <formula>NOT(ISERROR(SEARCH("YEL",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="17" stopIfTrue="1" operator="containsText" text="BLU">
+      <formula>NOT(ISERROR(SEARCH("BLU",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="18" stopIfTrue="1" operator="containsText" text="BRN">
+      <formula>NOT(ISERROR(SEARCH("BRN",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="19" stopIfTrue="1" operator="containsText" text="G/Y">
+      <formula>NOT(ISERROR(SEARCH("G/Y",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="20" stopIfTrue="1" operator="containsText" text="GRN">
+      <formula>NOT(ISERROR(SEARCH("GRN",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="21" stopIfTrue="1" operator="containsText" text="GRY">
+      <formula>NOT(ISERROR(SEARCH("GRY",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="22" stopIfTrue="1" operator="containsText" text="ORG">
+      <formula>NOT(ISERROR(SEARCH("ORG",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="23" stopIfTrue="1" operator="containsText" text="PNK">
+      <formula>NOT(ISERROR(SEARCH("PNK",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="24" stopIfTrue="1" operator="containsText" text="SKY">
+      <formula>NOT(ISERROR(SEARCH("SKY",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="25" stopIfTrue="1" operator="containsText" text="VLT">
+      <formula>NOT(ISERROR(SEARCH("VLT",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.1" right="0.1" top="0.1" bottom="0.13" header="0.3" footer="0"/>
+  <pageSetup paperSize="9" scale="68" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update-SD Calc for PD
</commit_message>
<xml_diff>
--- a/bin/Debug/Template/SDCalcForProduction_Template.xlsx
+++ b/bin/Debug/Template/SDCalcForProduction_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Current Works\MC-Dept-App\bin\Debug\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272C45EB-3E38-4246-9D22-5B16197BF9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2729454-697D-4F68-A870-E0E0FAE985FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{14D0DD05-F513-4696-888A-6119A7C86A21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{14D0DD05-F513-4696-888A-6119A7C86A21}"/>
   </bookViews>
   <sheets>
     <sheet name="RachhanSystem" sheetId="1" r:id="rId1"/>
@@ -950,6 +950,157 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1343024</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>542924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2362199</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>304799</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEB09916-810F-9B62-9780-11DFCC9F0441}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2600324" y="1057274"/>
+          <a:ext cx="1019175" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="km-KH" sz="1200" b="0" u="sng">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Khmer OS Battambang" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+              <a:cs typeface="Khmer OS Battambang" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t>ឈ្មោះម៉ាស៊ីន</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2324101</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>542924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1752601</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>304799</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="$C$3">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CF070A6-9C6A-8FAF-C3DB-95288E297B24}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3581401" y="1057274"/>
+          <a:ext cx="3162300" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:fld id="{F5706A2C-8DD9-4CEE-AABC-585E317E0543}" type="TxLink">
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Khmer OS Battambang" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Khmer OS Battambang" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t> ៖ </a:t>
+          </a:fld>
+          <a:endParaRPr lang="en-US" sz="1600">
+            <a:latin typeface="Khmer OS Battambang" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+            <a:cs typeface="Khmer OS Battambang" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1285,9 +1436,9 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1318,6 +1469,10 @@
         <f>IF(A3&lt;&gt;""," ៖ "&amp;TEXT(A3,"dd-MM-yyyy")," ៖ ")</f>
         <v xml:space="preserve"> ៖ </v>
       </c>
+      <c r="C3" s="2" t="str">
+        <f>IF(C4&lt;&gt;""," ៖ "&amp;C4," ៖ ")</f>
+        <v xml:space="preserve"> ៖ </v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="26.25" customHeight="1" thickBot="1">
       <c r="A4" s="1"/>
@@ -1325,6 +1480,7 @@
         <f>IF(A4&lt;&gt;""," ៖ "&amp;A4," ៖ ")</f>
         <v xml:space="preserve"> ៖ </v>
       </c>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" ht="23.25">
       <c r="A5" s="3" t="s">
@@ -1377,9 +1533,9 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G1"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1396,7 +1552,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="50.25" customHeight="1">
       <c r="A1" s="29" t="str">
-        <f>IF(RachhanSystem!A4&lt;&gt;"",RachhanSystem!A4,"")</f>
+        <f>IF(RachhanSystem!A4&lt;&gt;"",RachhanSystem!A4&amp;"( "&amp;RachhanSystem!C4&amp;" )","")</f>
         <v/>
       </c>
       <c r="B1" s="29"/>

</xml_diff>